<commit_message>
i18n(CWL): update loc entries
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881E33AA-CDFE-4B22-B90D-80D955D7EA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32A71CC-84E0-438A-81FC-EF2441F4524B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1147,6 +1147,18 @@
       <t xml:space="preserve"> {0}, {1}
 {2}</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>removed invalid quest id: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已移除无效任务: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_post_cleanup_quest</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1565,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2181,6 +2193,18 @@
         <v>148</v>
       </c>
     </row>
+    <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D39">
     <sortCondition ref="A4:A39"/>

</xml_diff>

<commit_message>
fix(CWL): use `SafeQueryTypes` for decltype
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3AD686-615E-41FC-9C6E-04E34E601E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0386ED04-B1C4-414E-AE77-94CB8EF6A635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="155">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1158,6 +1158,83 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> {2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_decltype_missing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>failed to query decltype from mod: {0} -&gt; {1}
+it might've failed to load or is missing (transitive) dependencies
+this is not an exception from CWL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法查询MOD声明类型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: {0} -&gt; {1}  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>或许它未能加载或缺少（传递）依赖项</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">这并不是一个 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">CWL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>异常</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1166,7 +1243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1247,6 +1324,12 @@
     <font>
       <sz val="15.8"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15.8"/>
+      <name val="微软雅黑"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
@@ -1577,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2205,6 +2288,18 @@
         <v>149</v>
       </c>
     </row>
+    <row r="53" spans="1:4" ht="93" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D39">
     <sortCondition ref="A4:A39"/>

</xml_diff>

<commit_message>
feat(CWL): custom merchant & stock
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F02D47D-BB4E-45FF-9481-9AC1F20D18DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDF4DAC-328A-4AC3-BB73-83704AAE5136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="176">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1201,12 +1201,6 @@
       <t xml:space="preserve"> {1}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_warn_empty_default</t>
-  </si>
-  <si>
-    <t>sheet is missing default entries (3rd row) and might be incompatible</t>
   </si>
   <si>
     <r>
@@ -1490,6 +1484,52 @@
   </si>
   <si>
     <t>这是最后一次警告此元素，后续异常将会被静默忽略</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_empty_default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheet is missing default entries (3rd row) and might be incompatible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_stock_file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>failed to read stock file for merchant id: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法为商人:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>加载自定义库存</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1923,10 +1963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="C54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2085,7 +2125,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>110</v>
@@ -2454,21 +2494,21 @@
         <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
@@ -2487,10 +2527,10 @@
         <v>92</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2622,15 +2662,28 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>164</v>
+    </row>
+    <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(CWL): add partial docs & reformat
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FDB40-83DE-43D1-A57B-9F0911A04CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504D39E8-9FB0-46D0-BF7E-3BD81A27ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1943,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat(CWL): mod integrity check
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504D39E8-9FB0-46D0-BF7E-3BD81A27ED1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8458467-270E-43FE-A1DA-983FD437811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="182">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1495,6 +1495,60 @@
         <family val="3"/>
       </rPr>
       <t>: {1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_missing_mods</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_missing_mods_yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_missing_mods_no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>继续游玩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不保存并返回至标题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>現在のセーブから欠落しているMOD：
+{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>セーブせずに終了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>プレイを続ける</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当前存档中缺失的模组：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+{0}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1941,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="D53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2649,12 +2703,42 @@
       <c r="C59" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
+    <row r="60" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): `EffectSetting` loader (`guns` only for now)
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5685A9C-ADBE-4706-8A8E-DC49F799EC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19202A-9F74-44DB-B4F2-0847918433A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="191">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -414,10 +414,6 @@
   </si>
   <si>
     <t>为音频 {0} 生成了默认元数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>预加载称号 &gt; {0}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1568,9 +1564,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[CWL] {0} がロードされました。</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="15.8"/>
@@ -1636,7 +1629,69 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[CWL] {0} がロードされました。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>[CWL] 音声 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_effect_loaded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>预加载称号</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loaded EffectSetting/{0}: {1} &gt; {2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已加载效果数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>/{0}: {1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; {2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1773,7 +1828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1807,9 +1862,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2091,10 +2143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2170,10 +2222,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2194,7 +2246,7 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>85</v>
@@ -2253,7 +2305,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>88</v>
@@ -2261,14 +2313,14 @@
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2277,7 +2329,7 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>89</v>
@@ -2289,7 +2341,7 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>80</v>
@@ -2337,7 +2389,7 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>68</v>
@@ -2349,7 +2401,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>69</v>
@@ -2371,7 +2423,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>93</v>
@@ -2379,14 +2431,14 @@
     </row>
     <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -2395,10 +2447,10 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2407,7 +2459,7 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>94</v>
@@ -2419,7 +2471,7 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>70</v>
@@ -2457,8 +2509,8 @@
       <c r="C30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>95</v>
+      <c r="D30" s="6" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2470,7 +2522,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2482,7 +2534,7 @@
         <v>38</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2494,7 +2546,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2506,7 +2558,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -2518,7 +2570,7 @@
         <v>42</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2530,7 +2582,7 @@
         <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2539,10 +2591,10 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -2551,7 +2603,7 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>71</v>
@@ -2563,10 +2615,10 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2587,10 +2639,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2602,7 +2654,7 @@
         <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2614,75 +2666,75 @@
         <v>67</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="116.25" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="8" customFormat="1" ht="209.25" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -2704,159 +2756,197 @@
         <v>76</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
+    </row>
+    <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C63" s="9" t="s">
+    </row>
+    <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="C64" s="9" t="s">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D64" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
chore(CWL): upload assets & cleanups
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAF44DD-51AA-4CBD-9CF6-73DB0F4448FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0558B886-E713-43CB-8D43-0DA8F453ECCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="224">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1767,12 +1767,368 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>cwl_log_processor_add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added processor {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注册处理器 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_bgm_clip_replace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_bgm_id_collision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assigned row based id: {0} to BGM: {1}, excplicit id is preferred to avoid BGM lookup collision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_bgm_added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added new BGM: {0} {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BGM global replacement: {0}, {1} =&gt; {2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BGM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全局替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}, {1} =&gt; {2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_error_source_rethrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_error_source_rethrow_def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>, SourceData begins at the 4th row. 3rd row is expected to be the default value row.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>, default:{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_error_source_rethrow_row</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>BGM {</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>正在使用行序号作为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ID: {1}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>建议手动设置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以避免可能的冲突。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加了新 BGM {0} {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_playlist_empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skipped empty playlist {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_playlist_added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added {0}, merge {1}, remove {2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">#{0}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>列</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">#{1}/{2}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>类型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">:{3}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>值:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{4}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+row#{0}, cell#{1}/{2}, expected:{3}, raw:{4}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>源表数据从第四行开始。第三行是默认值。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>默认值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>:{0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>跳过空白播放列表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已添加播放列表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {0}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">新增 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{1}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">移除 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1874,6 +2230,13 @@
       <name val="Cascadia Code"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="15.8"/>
+      <color rgb="FF89CA78"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1895,7 +2258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1936,7 +2299,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2219,17 +2585,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52.375" style="9" customWidth="1"/>
     <col min="2" max="2" width="20.375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="91.625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="93.75" style="9" customWidth="1"/>
     <col min="4" max="4" width="156.125" style="7" customWidth="1"/>
     <col min="5" max="16384" width="9" style="7"/>
   </cols>
@@ -3012,29 +3378,125 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B67" s="4"/>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="4" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+      <c r="A68" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="B68" s="4"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
+      <c r="C68" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="A69" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): safe load quest deliver hat noa doesn't check
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98735158-A525-481A-BEED-8EC777814455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536763CD-5877-47F9-ADBA-FA54AD4335B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="236">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1748,10 +1748,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>assigned row based id: {0} to BGM: {1}, excplicit id is preferred to avoid BGM lookup collision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_log_bgm_added</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2175,6 +2171,100 @@
   </si>
   <si>
     <t>详细：{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assigned row based id: {1} to BGM: {0}, excplicit id is preferred to avoid BGM lookup collision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_quest_id_thing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quest {0} is trying to use invalid id: "{1}"
+CWL kept the game going by replacing it with "{2}"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">任务 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用了无效的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>: "{1}"
+CWL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">将其替换为了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>"{2}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>来保持游戏进行。</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2641,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3426,10 +3516,10 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3462,10 +3552,10 @@
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -3474,125 +3564,131 @@
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="D79" s="14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
+    </row>
+    <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
+      <c r="C80" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): purge invalid items when quest board queries
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536763CD-5877-47F9-ADBA-FA54AD4335B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBBCD19-2641-46A8-BB03-6B666648DBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="239">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2264,6 +2264,53 @@
         <charset val="134"/>
       </rPr>
       <t>来保持游戏进行。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_quest_id_thing2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWL purged invalid item id: "{0}"
+{1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>CWL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>移除了无效的物品</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>: "{0}"
+{1}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2732,7 +2779,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3690,11 +3737,17 @@
         <v>235</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+    <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="C81" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): exception handler & stackframe analyzer
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE00D4E0-A8C3-4470-9A63-98A6BDE8B668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82469EE2-D30E-4D34-B334-FBB8FA45C19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="260">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2537,12 +2537,36 @@
     <t>cwl_ui_hover_close</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>cwl_ui_exception_analyzing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_exception_analyze</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;分析スタックフレーム中…&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;可分析スタックフレーム&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;可分析栈帧&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;分析栈帧中…&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2651,6 +2675,12 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="15.8"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2672,7 +2702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2718,6 +2748,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3001,8 +3034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4032,17 +4065,29 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A87" s="4"/>
+    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>255</v>
+      </c>
       <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
+      <c r="C87" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A88" s="4"/>
+      <c r="A88" s="4" t="s">
+        <v>254</v>
+      </c>
       <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
+      <c r="C88" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): `CustomMerchant` API rework
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC92AB36-87D5-4FF4-9A82-567F8130CCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E8566B-DB13-455B-9975-94984E3117FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5205" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="272">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1652,26 +1652,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>加载音频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>loaded EffectSetting</t>
     </r>
     <r>
@@ -2130,10 +2110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>随机排列：{0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="15.8"/>
@@ -2484,45 +2460,6 @@
         <charset val="134"/>
       </rPr>
       <t>詳細情報を表示</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>右クリック</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>閉じる</t>
     </r>
     <r>
       <rPr>
@@ -2645,6 +2582,160 @@
       </rPr>
       <t>个专属元素</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>预加载音频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机：{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>右クリック</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>閉じる</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_stock_merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_stock_add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>added new stock: {0} to character id: {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">已添加商人库存 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">至 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">已合并商人库存 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">至 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merged stock: {0} into character id: {1}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3118,10 +3209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3740,7 +3831,7 @@
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>185</v>
@@ -3881,10 +3972,10 @@
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3893,10 +3984,10 @@
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -3905,10 +3996,10 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3917,299 +4008,371 @@
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="18" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D88" s="16" t="s">
         <v>256</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>265</v>
+        <v>261</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A91" s="4"/>
+      <c r="A91" s="4" t="s">
+        <v>266</v>
+      </c>
       <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="C91" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A92" s="4"/>
+      <c r="A92" s="4" t="s">
+        <v>267</v>
+      </c>
       <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
+      <c r="C92" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+    </row>
+    <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): `CwlContextMenu` for popper events
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7803B9-B51C-4241-A457-B4DF1D2ED53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D6B9AF-AD0D-46A0-82A5-02D3C377D17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51390" yWindow="5535" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="15" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="302">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2760,6 +2760,182 @@
   </si>
   <si>
     <t>无法为物品 {1} 应用转换规则 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_stub_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CWL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>单帧信息</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_stub_header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>占比</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>平均帧</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ms</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CWL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>単フレーム情報</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>占有率</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>平均フレーム</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ms</t>
+    </r>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_hide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>プレイリストを見る</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>プレイリストを隠す</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次の曲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_last</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前の曲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_shuffle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>シャッフル</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_rebuild</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>プレイリストデータの再構築</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重载列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一首</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上一首</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机播放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3242,10 +3418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4372,52 +4548,202 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="4"/>
+      <c r="A95" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
+      <c r="C95" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A96" s="4"/>
+      <c r="A96" s="4" t="s">
+        <v>280</v>
+      </c>
       <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-    </row>
-    <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A97" s="4"/>
+      <c r="C96" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>284</v>
+      </c>
       <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-    </row>
-    <row r="98" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A98" s="4"/>
+      <c r="C97" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>285</v>
+      </c>
       <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
+      <c r="C98" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A99" s="4"/>
+      <c r="A99" s="4" t="s">
+        <v>288</v>
+      </c>
       <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-    </row>
-    <row r="100" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A100" s="4"/>
+      <c r="C99" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>290</v>
+      </c>
       <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
+      <c r="C100" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A101" s="4"/>
+      <c r="A101" s="4" t="s">
+        <v>292</v>
+      </c>
       <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-    </row>
-    <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A102" s="4"/>
+      <c r="C101" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>294</v>
+      </c>
       <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
+      <c r="C102" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): `CustomConverter` API rework
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D6B9AF-AD0D-46A0-82A5-02D3C377D17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBB4A06-25DE-4C67-8A56-738F738591A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="15" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="305">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2936,6 +2936,18 @@
   </si>
   <si>
     <t>隐藏列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_converter_reload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>再構築</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重载规则</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3420,8 +3432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4644,10 +4656,16 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A103" s="4"/>
+      <c r="A103" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
+      <c r="C103" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): MMB to hide exception for `ExceptionProfile`
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBB4A06-25DE-4C67-8A56-738F738591A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE62CF5A-6DD2-4BBB-83D8-B5A428B1175B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="15" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2409,68 +2409,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标右键</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关闭</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>詳細情報を表示</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>cwl_ui_hover_close</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2609,46 +2547,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>右クリック</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>閉じる</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_log_stock_merge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2948,6 +2846,179 @@
   </si>
   <si>
     <t>重载规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>詳細情報を表示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>マウス右クリック</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>閉じる</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;
+&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウス中クリック</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>閉じて再表示しない</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标右键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;
+&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标中键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭且不再显示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3432,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4208,7 +4279,7 @@
         <v>190</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -4352,7 +4423,7 @@
         <v>222</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4444,227 +4515,227 @@
         <v>246</v>
       </c>
       <c r="B85" s="4"/>
-      <c r="C85" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
+      <c r="B87" s="4"/>
+      <c r="C87" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="D87" s="16" t="s">
-        <v>255</v>
+      <c r="D87" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>256</v>
+      <c r="D88" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B91" s="4"/>
-      <c r="C91" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>270</v>
+      <c r="C91" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B92" s="4"/>
-      <c r="C92" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D92" s="12" t="s">
-        <v>269</v>
+      <c r="C92" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B93" s="4"/>
-      <c r="C93" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>274</v>
+      <c r="C93" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="18" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="18" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore(CWL): cleanups & bump version
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A0C36-B9DB-420B-81AB-21E7F4C016E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F2B99-2DB9-4E03-A7C8-C33122F39721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="15" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13200" yWindow="3585" windowWidth="28185" windowHeight="16695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="323">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -386,10 +386,6 @@
   </si>
   <si>
     <t>无法导入 {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加冒险者: {0} 至 {1}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1087,26 +1083,6 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>添加角色</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>: {0} to {1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
         <rFont val="微软雅黑"/>
         <family val="2"/>
         <charset val="134"/>
@@ -3075,6 +3051,127 @@
   </si>
   <si>
     <t>変換器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_deduplicate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>de-duplicated rows: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除重复行: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_unique_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} row count {1} | unique count {2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>行数 {1} | 去重 {2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>添加冒险者</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>至</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>添加角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>至</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_spatial_gen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instantiating new zone {0} / {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成新区域 {0} / {1}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3569,7 +3666,7 @@
   <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3645,10 +3742,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3669,7 +3766,7 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>85</v>
@@ -3728,22 +3825,22 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>88</v>
+        <v>140</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>163</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3752,10 +3849,10 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3764,7 +3861,7 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>80</v>
@@ -3791,7 +3888,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3803,7 +3900,7 @@
         <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3812,7 +3909,7 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>68</v>
@@ -3824,7 +3921,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>69</v>
@@ -3838,7 +3935,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3846,22 +3943,22 @@
         <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -3870,10 +3967,10 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3882,10 +3979,10 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3894,7 +3991,7 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>70</v>
@@ -3933,7 +4030,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3945,7 +4042,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3957,7 +4054,7 @@
         <v>38</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3969,7 +4066,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3981,7 +4078,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -3993,7 +4090,7 @@
         <v>42</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4005,7 +4102,7 @@
         <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4014,10 +4111,10 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -4026,7 +4123,7 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>71</v>
@@ -4038,10 +4135,10 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4062,10 +4159,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4077,7 +4174,7 @@
         <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4089,75 +4186,75 @@
         <v>67</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="116.25" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="8" customFormat="1" ht="209.25" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4179,683 +4276,701 @@
         <v>76</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>189</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="18" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A107" s="4"/>
+      <c r="A107" s="4" t="s">
+        <v>312</v>
+      </c>
       <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
+      <c r="C107" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
+      <c r="A108" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
+      <c r="C108" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A109" s="4"/>
+      <c r="A109" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="C109" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A110" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): improve `ExceptionProfile` hinting and colors
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8138BC-A815-460D-BB30-6F7DEF21D59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF249057-8B34-4010-A295-7CFE074E66B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="3405" windowWidth="31380" windowHeight="16695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14940" yWindow="1545" windowWidth="31380" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2275,22 +2275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;分析スタックフレーム中…&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;可分析スタックフレーム&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;可分析栈帧&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;分析栈帧中…&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_error_merge_god_elements</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2700,104 +2684,6 @@
   </si>
   <si>
     <t>重载规则</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>詳細情報を表示</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>マウス右クリック</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>閉じる</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;
-&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>マウス中クリック</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>閉じて再表示しない</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3327,6 +3213,230 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> {2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标悬浮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>查看详细信息</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分析栈帧中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>…&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>詳細を表示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウスの右ボタン</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>閉じる</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;
+&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウスの中ボタン</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>閉じて今後表示しない</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウスを乗せて</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>詳細を表示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>スタックフレーム分析中…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3821,8 +3931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3984,7 +4094,7 @@
         <v>138</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -3996,7 +4106,7 @@
         <v>136</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4513,10 +4623,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4597,7 +4707,7 @@
         <v>186</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -4678,10 +4788,10 @@
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4741,7 +4851,7 @@
         <v>216</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4828,340 +4938,340 @@
         <v>239</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>240</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="51" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>242</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>244</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>246</v>
+        <v>330</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>248</v>
+        <v>327</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="14" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="14" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="20" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="93" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="3" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat(CWL): `equip_item` & value stack drama expansions
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620959EA-68A6-4537-97C3-9AAF47CD7FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30376F8-3D71-47C4-ACE1-08CD369ECFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2805" yWindow="1230" windowWidth="31380" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="347">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3473,6 +3473,73 @@
   </si>
   <si>
     <t>已恢复角色数据 {0} 至 {1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_yes</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_no</t>
+  </si>
+  <si>
+    <t>恢复角色数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保持现状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>下列角色数据可供恢复:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+{0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>次のキャラクターのデータが復元可能です：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+{0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>キャラクターデータを復元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>このままにする</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3628,7 +3695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3683,6 +3750,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3966,8 +4036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D114" sqref="A114:D114"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115:C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5333,23 +5403,41 @@
         <v>337</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A115" s="4"/>
+    <row r="115" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-    </row>
-    <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A116" s="4"/>
+      <c r="C115" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="D115" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>339</v>
+      </c>
       <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
-    </row>
-    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="4"/>
+      <c r="C116" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>340</v>
+      </c>
       <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
+      <c r="C117" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A118" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): allow custom BGM dropped in tapes
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30376F8-3D71-47C4-ACE1-08CD369ECFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D18849-7030-469B-9B99-6FF1947C32D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="1230" windowWidth="31380" windowHeight="18825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="1275" windowWidth="31380" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="350">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2853,10 +2853,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>清理乞丐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="15.8"/>
@@ -3540,6 +3536,22 @@
   </si>
   <si>
     <t>このままにする</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_add_known</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加至留声机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓄音機に追加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清理乞丐（小鸡）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4036,8 +4048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115:C117"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4199,7 +4211,7 @@
         <v>138</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -4211,7 +4223,7 @@
         <v>136</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4728,10 +4740,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>324</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5049,7 +5061,7 @@
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>241</v>
@@ -5061,7 +5073,7 @@
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>292</v>
@@ -5073,10 +5085,10 @@
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5085,10 +5097,10 @@
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -5261,14 +5273,14 @@
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5301,149 +5313,155 @@
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>299</v>
+        <v>349</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D107" s="16" t="s">
         <v>305</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="D109" s="16" t="s">
         <v>313</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D110" s="12" t="s">
         <v>316</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="93" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D112" s="10" t="s">
         <v>322</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D113" s="12" t="s">
         <v>333</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D114" s="16" t="s">
         <v>336</v>
-      </c>
-      <c r="D114" s="16" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D117" s="14" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A118" s="4"/>
       <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
+      <c r="C118" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A119" s="4"/>

</xml_diff>

<commit_message>
feat(CWL): better drama loc support
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819CB670-D92D-4D44-944A-19A80CCD0B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E74364A-B797-4237-9599-947C68AB6ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="1170" windowWidth="34710" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8325" yWindow="990" windowWidth="37590" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -3473,6 +3473,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>removed {0} chicken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清理小鸡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ひよこの掃除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="15.8"/>
@@ -3488,24 +3500,7 @@
         <rFont val="Cascadia Code"/>
         <family val="3"/>
       </rPr>
-      <t>, &lt;s&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>浪汉</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;/s&gt;</t>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -3542,18 +3537,6 @@
       </rPr>
       <t>只野鸡</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>removed {0} chicken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清理小鸡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ひよこの掃除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4048,7 +4031,7 @@
   <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5312,10 +5295,10 @@
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5372,10 +5355,10 @@
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="93" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat(CWL): added fix for missing mod elements
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E74364A-B797-4237-9599-947C68AB6ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEFFA4E-7B6B-43D8-8316-349B0843158E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8325" yWindow="990" windowWidth="37590" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8670" yWindow="1335" windowWidth="37590" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="356">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3536,6 +3536,72 @@
         <charset val="134"/>
       </rPr>
       <t>只野鸡</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_fix_actCombat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_fix_listAbility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>角色 {1} 移除了无效的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> actCombat ID: {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色 {1} 移除了无效的 listAbility ID: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">removed invalid actCombat ID: {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>from {1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">removed invalid listAbility ID: {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>from {1}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4030,8 +4096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5446,16 +5512,28 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A119" s="4"/>
+      <c r="A119" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
+      <c r="C119" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A120" s="4"/>
+      <c r="A120" s="2" t="s">
+        <v>351</v>
+      </c>
       <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
+      <c r="C120" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): add line number to build list
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD212CE-F982-477E-81D7-80C5FD3BE2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80961395-4DA2-4449-BF77-65A2230CA0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="6105" windowWidth="25395" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="3255" windowWidth="25395" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2428,10 +2428,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>重载列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>下一首</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2441,14 +2437,6 @@
   </si>
   <si>
     <t>随机播放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐藏列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3064,25 +3052,6 @@
   </si>
   <si>
     <t>cwl_warn_pop_talk_empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} attempts to pop empty text, CWL prevented it</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">{0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>试图发出空白文本喊叫, CWL制止了这个行为</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3544,8 +3513,39 @@
   </si>
   <si>
     <t>Error occurred during drama play!
-Please check the Player.log and mods.
+Please check Player.log and mods.
 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>试图发出空白文本喊叫, CWL取消了这个行为</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} attempts to pop empty text, CWL stopped it</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看播放列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏播放列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重载播放列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4039,8 +4039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="B89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4202,7 +4202,7 @@
         <v>138</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -4214,7 +4214,7 @@
         <v>136</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4592,10 +4592,10 @@
         <v>126</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4625,10 +4625,10 @@
         <v>135</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4731,10 +4731,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4896,10 +4896,10 @@
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>237</v>
@@ -5064,10 +5064,10 @@
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5076,10 +5076,10 @@
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5088,10 +5088,10 @@
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -5199,7 +5199,7 @@
         <v>269</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>283</v>
+        <v>353</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5211,7 +5211,7 @@
         <v>270</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>284</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5223,7 +5223,7 @@
         <v>272</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5235,7 +5235,7 @@
         <v>274</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5247,7 +5247,7 @@
         <v>276</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5259,223 +5259,223 @@
         <v>278</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>279</v>
+        <v>355</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="18" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>324</v>
+        <v>351</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="20" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="18" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="18" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D118" s="16" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="14" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="14" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build(CWL): separate build configs
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55845CEA-8D3A-490D-A6D1-D63F89BB1CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BCE10F-AE69-46B8-9F79-28F4CCF6F58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2925" windowWidth="32715" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19680" yWindow="3915" windowWidth="25725" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="356">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1221,10 +1221,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwl_log_finished_loading</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="15.8"/>
@@ -1343,21 +1339,6 @@
   </si>
   <si>
     <r>
-      <t>CWL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、OK！ &gt;_&lt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>音声</t>
     </r>
     <r>
@@ -1368,10 +1349,6 @@
       </rPr>
       <t xml:space="preserve"> {0}</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>感谢使用 CWL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3511,6 +3488,77 @@
       </rPr>
       <t xml:space="preserve"> {0}</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_finished_loading_stable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_finished_loading_nightly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CWL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、OK！ &gt;_&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;color=#21a366&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>安定版&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CWL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、OK！ &gt;_&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;color=#427ddc&gt;Nightly&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢使用 CWL &lt;color=#427ddc&gt;Nightly&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>感谢使用 CWL &lt;color=#21a366&gt;稳定版&lt;/color&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4030,10 +4078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="B57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4195,7 +4243,7 @@
         <v>136</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -4207,7 +4255,7 @@
         <v>134</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4397,7 +4445,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4585,10 +4633,10 @@
         <v>124</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4618,10 +4666,10 @@
         <v>133</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4648,14 +4696,14 @@
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4724,10 +4772,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4748,10 +4796,10 @@
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4759,7 +4807,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>169</v>
@@ -4789,674 +4837,686 @@
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>170</v>
+        <v>350</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>179</v>
+        <v>352</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>181</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>172</v>
+        <v>351</v>
       </c>
       <c r="B65" s="4"/>
-      <c r="C65" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="C65" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B66" s="4"/>
-      <c r="C66" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="C66" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B67" s="4"/>
-      <c r="C67" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>182</v>
+      <c r="C67" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>224</v>
+        <v>180</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>187</v>
       </c>
+    </row>
+    <row r="71" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="B71" s="4"/>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="D71" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="B73" s="4"/>
-      <c r="C73" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="C73" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>192</v>
       </c>
       <c r="B74" s="4"/>
-      <c r="C74" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>203</v>
+      <c r="C74" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>198</v>
+      <c r="A75" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
-        <v>200</v>
+      <c r="A76" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D77" s="16" t="s">
-        <v>246</v>
+        <v>198</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="B80" s="4"/>
-      <c r="C80" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>219</v>
+      <c r="C80" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>225</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="B82" s="4"/>
-      <c r="C82" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>229</v>
+      <c r="C82" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="D83" s="14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>234</v>
+    </row>
+    <row r="85" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>307</v>
+        <v>229</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="51" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>239</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>240</v>
+        <v>307</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>242</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
         <v>249</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A94" s="19" t="s">
-        <v>256</v>
+      <c r="A94" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="B94" s="4"/>
-      <c r="C94" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>258</v>
+      <c r="C94" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
-        <v>259</v>
+      <c r="A95" s="19" t="s">
+        <v>253</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>260</v>
+        <v>254</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B97" s="4"/>
+      <c r="C97" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="D97" s="16" t="s">
-        <v>345</v>
+      <c r="D97" s="15" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B99" s="4"/>
+      <c r="C99" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D98" s="14" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
+      <c r="B101" s="4"/>
+      <c r="C101" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="B99" s="4"/>
-      <c r="C99" s="16" t="s">
+      <c r="D101" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D99" s="14" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B100" s="4"/>
-      <c r="C100" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B102" s="4"/>
-      <c r="C102" s="18" t="s">
+      <c r="D102" s="14" t="s">
         <v>276</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B104" s="4"/>
+      <c r="C104" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" s="4"/>
+      <c r="C105" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A106" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B107" s="4"/>
+      <c r="C107" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B104" s="4"/>
-      <c r="C104" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A105" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D105" s="16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>301</v>
+      <c r="A109" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D110" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="D109" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B110" s="4"/>
-      <c r="C110" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B111" s="4"/>
-      <c r="C111" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>343</v>
+      <c r="C111" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
-        <v>312</v>
+      <c r="A112" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B113" s="4"/>
-      <c r="C113" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="D113" s="10" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="C113" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B114" s="4"/>
-      <c r="C114" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="D114" s="14" t="s">
+      <c r="C114" s="20" t="s">
         <v>318</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="18" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="D116" s="16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>331</v>
+        <v>320</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>321</v>
       </c>
       <c r="B117" s="4"/>
-      <c r="C117" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>333</v>
+      <c r="C117" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="14" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A119" s="21" t="s">
-        <v>348</v>
-      </c>
-      <c r="B119" s="21"/>
-      <c r="C119" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="D119" s="23" t="s">
-        <v>350</v>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A120" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B120" s="21"/>
+      <c r="C120" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(CWL): add a helper line explaining MissingMethodException
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EB9E3-8D43-43B5-AFEB-7BA840DFCDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20424D82-5BB4-4802-BF21-D8AAED3D3D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10800" yWindow="3285" windowWidth="29205" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="365">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3623,6 +3623,79 @@
         <family val="3"/>
       </rPr>
       <t>ID: {0} / {1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_missing_method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MOD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">は、お使いのゲームバージョンに対応していません。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>Mod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与您当前游戏版本不兼容。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+{0}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4144,10 +4217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5609,17 +5682,44 @@
         <v>361</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A123" s="21"/>
+    <row r="123" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B123" s="21"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="21"/>
+      <c r="C123" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A124" s="21"/>
+      <c r="A124" s="2"/>
       <c r="B124" s="21"/>
       <c r="C124" s="21"/>
       <c r="D124" s="21"/>
+    </row>
+    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A131" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): restore mod chara data if recoverable
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5E544-7EF1-461E-9F03-85C66E665A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085544B3-2F42-4FCF-91F8-468FF298D911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="3480" windowWidth="31395" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="3075" windowWidth="31395" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="362">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2963,85 +2963,6 @@
   </si>
   <si>
     <t>cwl_warn_pop_talk_empty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_log_chara_restore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>restored chara data {0} to {1}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已恢复角色数据 {0} 至 {1}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore</t>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore_yes</t>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore_no</t>
-  </si>
-  <si>
-    <t>恢复角色数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保持现状</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>下列角色数据可供恢复:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-{0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>次のキャラクターのデータが復元可能です：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-{0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>キャラクターデータを復元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>このままにする</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3866,6 +3787,35 @@
   </si>
   <si>
     <t>removed {0} character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_chara_restore</t>
+  </si>
+  <si>
+    <r>
+      <t>「</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>」のキャラデータを復元しました</t>
+    </r>
+  </si>
+  <si>
+    <t>已恢复角色数据 {0}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3873,7 +3823,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3996,12 +3946,6 @@
     </font>
     <font>
       <sz val="15.8"/>
-      <name val="Cascadia Code"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="15.8"/>
       <color rgb="FF000000"/>
       <name val="Cascadia Code"/>
       <family val="3"/>
@@ -4048,7 +3992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4102,18 +4046,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4396,10 +4337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4951,10 +4892,10 @@
         <v>124</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4984,10 +4925,10 @@
         <v>133</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5114,10 +5055,10 @@
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5155,26 +5096,26 @@
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5570,7 +5511,7 @@
         <v>264</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5582,7 +5523,7 @@
         <v>265</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5630,7 +5571,7 @@
         <v>273</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5675,10 +5616,10 @@
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="18" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5711,10 +5652,10 @@
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -5723,10 +5664,10 @@
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="3" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5735,188 +5676,152 @@
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B113" s="4"/>
+      <c r="C113" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4" t="s">
+      <c r="B114" s="4"/>
+      <c r="C114" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D114" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="D113" s="16" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="48.75" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="B114" s="4"/>
-      <c r="C114" s="20" t="s">
+    </row>
+    <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B115" s="4"/>
+      <c r="C115" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="D114" s="10" t="s">
+      <c r="D115" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B116" s="4"/>
+      <c r="C116" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B115" s="4"/>
-      <c r="C115" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B117" s="4"/>
-      <c r="C117" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="D117" s="16" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A117" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B117" s="20"/>
+      <c r="C117" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="D117" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B118" s="4"/>
-      <c r="C118" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>328</v>
+        <v>342</v>
+      </c>
+      <c r="B118" s="20"/>
+      <c r="C118" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="D118" s="22" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B119" s="4"/>
-      <c r="C119" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A120" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="B120" s="21"/>
+        <v>345</v>
+      </c>
+      <c r="B119" s="20"/>
+      <c r="C119" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="D119" s="22" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B120" s="20"/>
       <c r="C120" s="21" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B121" s="20"/>
+      <c r="C121" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="B121" s="21"/>
-      <c r="C121" s="22" t="s">
+      <c r="C122" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="D121" s="23" t="s">
+      <c r="D122" s="22" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B122" s="21"/>
-      <c r="C122" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="D122" s="23" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B123" s="21"/>
-      <c r="C123" s="22" t="s">
-        <v>361</v>
-      </c>
-      <c r="D123" s="22" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B124" s="21"/>
-      <c r="C124" s="22" t="s">
-        <v>364</v>
-      </c>
-      <c r="D124" s="23" t="s">
-        <v>365</v>
-      </c>
+    <row r="123" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A123" s="2"/>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21"/>
+    </row>
+    <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A124" s="2"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
     </row>
     <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C125" s="24" t="s">
-        <v>367</v>
-      </c>
-      <c r="D125" s="23" t="s">
-        <v>368</v>
-      </c>
+      <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
-      <c r="C126" s="22"/>
-      <c r="D126" s="22"/>
     </row>
     <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
-      <c r="C127" s="22"/>
-      <c r="D127" s="22"/>
     </row>
     <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
-    </row>
-    <row r="129" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A129" s="2"/>
-    </row>
-    <row r="130" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A130" s="2"/>
-    </row>
-    <row r="131" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A131" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): improve Chara Restore code
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085544B3-2F42-4FCF-91F8-468FF298D911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B957187-17AF-4898-89B8-FA1F24EE9430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="3075" windowWidth="31395" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10875" yWindow="2190" windowWidth="31395" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="371">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3816,6 +3816,37 @@
   </si>
   <si>
     <t>已恢复角色数据 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore</t>
+  </si>
+  <si>
+    <t>復元可能なキャラクター: {0}</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_yes</t>
+  </si>
+  <si>
+    <t>データの復元</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_no</t>
+  </si>
+  <si>
+    <t>無視して再生成</t>
+  </si>
+  <si>
+    <t>可以恢复的角色数据:
+{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恢复数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忽略并重新生成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3992,7 +4023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4055,6 +4086,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4337,10 +4371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="B95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5694,134 +5728,170 @@
         <v>361</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>309</v>
+        <v>362</v>
       </c>
       <c r="B114" s="4"/>
-      <c r="C114" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="D114" s="16" t="s">
-        <v>310</v>
+      <c r="C114" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="D114" s="24" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
-        <v>314</v>
+      <c r="A115" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>316</v>
+        <v>365</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
-        <v>315</v>
+      <c r="A116" s="4" t="s">
+        <v>366</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="B117" s="20"/>
-      <c r="C117" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="D117" s="20" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B117" s="4"/>
+      <c r="C117" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B118" s="20"/>
-      <c r="C118" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="D118" s="22" t="s">
-        <v>344</v>
+        <v>314</v>
+      </c>
+      <c r="B118" s="4"/>
+      <c r="C118" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B119" s="20"/>
-      <c r="C119" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="D119" s="22" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>348</v>
+        <v>315</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A120" s="20" t="s">
+        <v>331</v>
       </c>
       <c r="B120" s="20"/>
-      <c r="C120" s="21" t="s">
-        <v>349</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="C120" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B121" s="20"/>
       <c r="C121" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B122" s="20"/>
+      <c r="C122" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="D122" s="22" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B123" s="20"/>
+      <c r="C123" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B124" s="20"/>
+      <c r="C124" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="D121" s="22" t="s">
+      <c r="D124" s="22" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C122" s="23" t="s">
+      <c r="C125" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="D122" s="22" t="s">
+      <c r="D125" s="22" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A123" s="2"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="21"/>
-    </row>
-    <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A124" s="2"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="21"/>
-    </row>
-    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="2"/>
     </row>
     <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
     </row>
     <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="21"/>
     </row>
     <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A131" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
build(CWL): update for 23.200 Stable
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB13A0A-51D0-4452-870D-19725F027E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61ABD57-BBFD-45D9-921B-BAD625C592FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3030" windowWidth="31395" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11010" yWindow="2865" windowWidth="23100" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -3419,8 +3419,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>MOD</t>
+    <t>cwl_warn_duplicate_cwl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CWL</t>
     </r>
     <r>
       <rPr>
@@ -3430,25 +3434,431 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">は、お使いのゲームバージョンに対応していません。
+      <t>のバージョンが</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>つ見つかりました！
+お使いのゲームに合ったバージョンのみを使用してください。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>发现了两个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>CWL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>版本！</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
         <sz val="15.8"/>
         <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>请仅使用与您的游戏相匹配的版本。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_callstack</t>
+  </si>
+  <si>
+    <r>
+      <t>エラーが発生した時点でのアプリの動作</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最も新しいものが一番上です</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>导致此错误的事件顺序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最后的事件在最上方</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>艾琳大地</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>浪鸡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">成群。清理了 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个角色</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>removed {0} character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_chara_restore</t>
+  </si>
+  <si>
+    <r>
+      <t>「</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
         <rFont val="Cascadia Code"/>
         <family val="3"/>
       </rPr>
       <t>{0}</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>」のキャラデータを復元しました</t>
+    </r>
+  </si>
+  <si>
+    <t>已恢复角色数据 {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore</t>
+  </si>
+  <si>
+    <t>復元可能なキャラクター: {0}</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_yes</t>
+  </si>
+  <si>
+    <t>データの復元</t>
+  </si>
+  <si>
+    <t>cwl_ui_chara_restore_no</t>
+  </si>
+  <si>
+    <t>無視して再生成</t>
+  </si>
+  <si>
+    <t>可以恢复的角色数据:
+{0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恢复数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忽略并重新生成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法生成人物</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>failed to create character {0}
+{1}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无法添加物品</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>至</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {1}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+{2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>failed to add thing:{0} to {1}
+{2}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_invalid_hobby</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="15.8"/>
         <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已将角色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> {1} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的无效</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Hobby {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>移除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>キャラクター {1} の無効なHobby {0} を削除しました</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=#d343f7&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
@@ -3473,6 +3883,15 @@
         <charset val="134"/>
       </rPr>
       <t>与您当前游戏版本不兼容。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;/color&gt;</t>
     </r>
     <r>
       <rPr>
@@ -3488,12 +3907,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwl_warn_duplicate_cwl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>CWL</t>
+    <r>
+      <t>&lt;color=#d343f7&gt;MOD</t>
     </r>
     <r>
       <rPr>
@@ -3503,7 +3918,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>のバージョンが</t>
+      <t>は、お使いのゲームバージョンに対応していません。</t>
     </r>
     <r>
       <rPr>
@@ -3512,7 +3927,7 @@
         <rFont val="Cascadia Code"/>
         <family val="3"/>
       </rPr>
-      <t>2</t>
+      <t>&lt;/color&gt;</t>
     </r>
     <r>
       <rPr>
@@ -3521,48 +3936,6 @@
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
-      </rPr>
-      <t>つ見つかりました！
-お使いのゲームに合ったバージョンのみを使用してください。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>发现了两个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>CWL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>版本！</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -3571,353 +3944,11 @@
       <rPr>
         <sz val="15.8"/>
         <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>请仅使用与您的游戏相匹配的版本。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_callstack</t>
-  </si>
-  <si>
-    <r>
-      <t>エラーが発生した時点でのアプリの動作</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>最も新しいものが一番上です</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>):</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>导致此错误的事件顺序</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>最后的事件在最上方</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>):</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>艾琳大地</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>浪鸡</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">成群。清理了 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个角色</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>removed {0} character</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_log_chara_restore</t>
-  </si>
-  <si>
-    <r>
-      <t>「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
         <rFont val="Cascadia Code"/>
         <family val="3"/>
       </rPr>
       <t>{0}</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>」のキャラデータを復元しました</t>
-    </r>
-  </si>
-  <si>
-    <t>已恢复角色数据 {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore</t>
-  </si>
-  <si>
-    <t>復元可能なキャラクター: {0}</t>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore_yes</t>
-  </si>
-  <si>
-    <t>データの復元</t>
-  </si>
-  <si>
-    <t>cwl_ui_chara_restore_no</t>
-  </si>
-  <si>
-    <t>無視して再生成</t>
-  </si>
-  <si>
-    <t>可以恢复的角色数据:
-{0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>恢复数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>忽略并重新生成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>无法生成人物</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>: {0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>failed to create character {0}
-{1}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>无法添加物品</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>至</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {1}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-{2}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>failed to add thing:{0} to {1}
-{2}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_warn_invalid_hobby</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>已将角色</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {1} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的无效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Hobby {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>移除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>キャラクター {1} の無効なHobby {0} を削除しました</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4444,8 +4475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4521,10 +4552,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4938,10 +4969,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5757,10 +5788,10 @@
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -5789,50 +5820,50 @@
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
@@ -5907,50 +5938,50 @@
         <v>343</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>344</v>
       </c>
       <c r="B123" s="20"/>
       <c r="C123" s="21" t="s">
-        <v>345</v>
+        <v>373</v>
       </c>
       <c r="D123" s="21" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B124" s="20"/>
       <c r="C124" s="21" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D124" s="22" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C125" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="D125" s="22" t="s">
         <v>350</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="D125" s="22" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C126" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="C126" s="23" t="s">
-        <v>373</v>
-      </c>
       <c r="D126" s="22" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat(CWL): test incompatible patches for exception profile
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343D9748-8912-477A-87D8-5ABFE8D876BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED5427-70C7-4174-ABD9-59CB1CA942E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9945" yWindow="2400" windowWidth="23100" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="377">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3971,6 +3971,57 @@
       <t>个供奉倍率</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_invalid_patch</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=#d343f7&gt;(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>互換性なし</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>)&lt;/color&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=#d343f7&gt;(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不兼容</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>)&lt;/color&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4496,8 +4547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6006,9 +6057,15 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A127" s="2"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="21"/>
+      <c r="A127" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="D127" s="21" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>

</xml_diff>

<commit_message>
feat!(CWL): avoid using Elin excel parser if cache present
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C6D5FD-F397-433F-8F07-1B3C586B4690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58AB6BD-C767-4EF7-AE35-546451E8E7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="4530" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18630" yWindow="3570" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="389">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -358,10 +358,6 @@
   </si>
   <si>
     <t>添加物品: {0},  x{1} 至 {2}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工作簿: {0}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3765,6 +3761,315 @@
         <family val="3"/>
         <charset val="128"/>
       </rPr>
+      <t>マウスを乗せて</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>詳細を表示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=blue&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标悬浮</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>查看详细信息</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_cache_gen</t>
+  </si>
+  <si>
+    <t>cwl_log_cache_detail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成されたソースキャッシュは、ロード時間を短縮します。
+次の生成：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">日
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>キャッシュ内のブロブ数：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>キャッシュの合計サイズ：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>缓存块计数：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>缓存总大小：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已生成源表缓存以减少加载时间。
+下一次生成于：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">{0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">天
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{1}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_exception_copy</t>
+  </si>
+  <si>
+    <t>cwl_warn_drama_id_collision</t>
+  </si>
+  <si>
+    <t>Drama ID collision [{0}] =&gt; [{1}] at line#{2}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>剧情文本</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">冲突 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">[{0}] =&gt; [{1}] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位于行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>#{2}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=blue&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
       <t>マウスの右ボタン</t>
     </r>
     <r>
@@ -3783,6 +4088,46 @@
         <charset val="128"/>
       </rPr>
       <t>閉じる</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=purple&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウスの左ボタン</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>詳細をコピー</t>
     </r>
     <r>
       <rPr>
@@ -3836,11 +4181,11 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>マウスを乗せて</t>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标右键</t>
     </r>
     <r>
       <rPr>
@@ -3853,11 +4198,11 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>詳細を表示</t>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭</t>
     </r>
     <r>
       <rPr>
@@ -3871,73 +4216,33 @@
   </si>
   <si>
     <r>
-      <t>&lt;color=blue&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标悬浮</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>查看详细信息</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;/color&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=blue&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标右键</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关闭</t>
+      <t>&lt;color=purple&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标左键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>复制详情</t>
     </r>
     <r>
       <rPr>
@@ -3985,10 +4290,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwl_ui_cache_gen</t>
-  </si>
-  <si>
-    <t>cwl_log_cache_detail</t>
+    <t>cwl_log_workbook_cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>workbook-cache: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_workbook_prefetch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>workbook-prefetch: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -3998,232 +4313,74 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>生成されたソースキャッシュは、ロード時間を短縮します。
-次の生成：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">日
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>キャッシュ内のブロブ数：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{0}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>キャッシュの合計サイズ：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>缓存块计数：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{0}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>缓存总大小：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>已生成源表缓存以减少加载时间。
-下一次生成于：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">天
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_exception_copy</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=purple&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标左键</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>复制详情</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;/color&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=purple&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>マウスの左ボタン</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>詳細をコピー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;/color&gt;</t>
+      <t>工作簿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作簿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>缓存</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>): {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作簿(预载)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4232,7 +4389,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4380,6 +4537,40 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="15.8"/>
+      <color rgb="FFFFC000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15.8"/>
+      <color rgb="FFFFC000"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15.8"/>
+      <color theme="1"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="15.8"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="15.8"/>
+      <color theme="1"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4401,7 +4592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4468,6 +4659,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4749,10 +4949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="B117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4807,7 +5007,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4828,10 +5028,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4843,7 +5043,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4852,10 +5052,10 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -4867,7 +5067,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4878,7 +5078,7 @@
         <v>59</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4911,22 +5111,22 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4935,10 +5135,10 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4947,7 +5147,7 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>80</v>
@@ -4974,7 +5174,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4986,7 +5186,7 @@
         <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -4995,7 +5195,7 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>68</v>
@@ -5007,7 +5207,7 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>69</v>
@@ -5021,7 +5221,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5029,22 +5229,22 @@
         <v>62</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -5053,10 +5253,10 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5065,10 +5265,10 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5077,7 +5277,7 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>70</v>
@@ -5091,8 +5291,8 @@
       <c r="C28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>81</v>
+      <c r="D28" s="6" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5116,7 +5316,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5128,7 +5328,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5140,7 +5340,7 @@
         <v>38</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5152,7 +5352,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5164,7 +5364,7 @@
         <v>39</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5176,7 +5376,7 @@
         <v>42</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5188,7 +5388,7 @@
         <v>32</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5197,10 +5397,10 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
@@ -5209,7 +5409,7 @@
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>71</v>
@@ -5221,10 +5421,10 @@
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5245,10 +5445,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5260,7 +5460,7 @@
         <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5272,75 +5472,75 @@
         <v>67</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="93" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="8" customFormat="1" ht="186" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5351,7 +5551,7 @@
         <v>74</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5362,932 +5562,962 @@
         <v>76</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>283</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D60" s="10" t="s">
         <v>311</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68" s="16" t="s">
         <v>210</v>
-      </c>
-      <c r="D68" s="16" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D72" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D77" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>198</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D80" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="D81" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D82" s="12" t="s">
         <v>215</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="51" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
         <v>379</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D104" s="16" t="s">
         <v>262</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D105" s="16" t="s">
         <v>267</v>
-      </c>
-      <c r="D105" s="16" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D107" s="16" t="s">
         <v>276</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D108" s="12" t="s">
         <v>279</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D111" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D111" s="25" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="B112" s="4"/>
-      <c r="C112" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+      <c r="D112" s="12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="D113" s="24" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="D114" s="16" t="s">
-        <v>342</v>
+        <v>335</v>
+      </c>
+      <c r="D114" s="24" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="14" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B116" s="4"/>
+      <c r="C116" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B117" s="4"/>
+      <c r="C117" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D117" s="16" t="s">
         <v>286</v>
-      </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="D116" s="16" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B117" s="4"/>
-      <c r="C117" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A119" s="20" t="s">
+      <c r="A119" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B119" s="4"/>
+      <c r="C119" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A120" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B120" s="20"/>
+      <c r="C120" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="B119" s="20"/>
-      <c r="C119" s="20" t="s">
+      <c r="D120" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="D119" s="20" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B120" s="20"/>
-      <c r="C120" s="21" t="s">
-        <v>318</v>
-      </c>
-      <c r="D120" s="22" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B121" s="20"/>
       <c r="C121" s="21" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B122" s="20"/>
       <c r="C122" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="D122" s="21" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+      <c r="D122" s="22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B123" s="20"/>
       <c r="C123" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B124" s="20"/>
+      <c r="C124" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D124" s="22" t="s">
         <v>325</v>
       </c>
-      <c r="D123" s="22" t="s">
+    </row>
+    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
+      <c r="C125" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="C124" s="23" t="s">
+      <c r="D125" s="22" t="s">
         <v>328</v>
-      </c>
-      <c r="D124" s="22" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="D125" s="22" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C126" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="D126" s="22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C127" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="D127" s="21" t="s">
         <v>357</v>
       </c>
-      <c r="D126" s="21" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="B127" s="4"/>
-      <c r="C127" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A129" s="2"/>
-    </row>
-    <row r="130" spans="1:1" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A130" s="2"/>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B129" s="4"/>
+      <c r="C129" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A130" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B130" s="26"/>
+      <c r="C130" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A131" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="B131" s="26"/>
+      <c r="C131" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>388</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): add control buttons to BGM panel
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58AB6BD-C767-4EF7-AE35-546451E8E7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823B19AE-00D8-459C-A633-6C733127C199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18630" yWindow="3570" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="555" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="379">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1523,54 +1523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwl_bgm_shuffle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_bgm_stream</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffle: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>streaming: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>衔接：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_bgm_detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>detailed: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>详细：{0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>assigned row based id: {1} to BGM: {0}, excplicit id is preferred to avoid BGM lookup collision</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1877,10 +1829,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>随机：{0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_log_stock_merge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2099,22 +2047,6 @@
     </r>
   </si>
   <si>
-    <t>cwl_ui_bgm_view</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_bgm_hide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>プレイリストを見る</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>プレイリストを隠す</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_ui_bgm_next</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2143,19 +2075,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>プレイリストデータの再構築</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>下一首</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>上一首</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机播放</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2788,14 +2712,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>隐藏播放列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重载播放列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cwl_ui_sound_reload</t>
   </si>
   <si>
@@ -4383,6 +4299,32 @@
       <t>: {0}</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>詳細</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_view</t>
+  </si>
+  <si>
+    <t>プレイリストを見る</t>
   </si>
 </sst>
 </file>
@@ -4949,10 +4891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5028,10 +4970,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5114,7 +5056,7 @@
         <v>134</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
@@ -5126,7 +5068,7 @@
         <v>132</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5292,7 +5234,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5445,10 +5387,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="3" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5504,10 +5446,10 @@
         <v>122</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5537,10 +5479,10 @@
         <v>131</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5643,10 +5585,10 @@
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5667,10 +5609,10 @@
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5708,26 +5650,26 @@
     </row>
     <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5736,10 +5678,10 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="14" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5748,10 +5690,10 @@
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5760,10 +5702,10 @@
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
@@ -5784,7 +5726,7 @@
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>184</v>
@@ -5808,10 +5750,10 @@
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="3" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
@@ -5862,661 +5804,625 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>194</v>
+    <row r="77" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="B77" s="4"/>
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D77" s="16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>195</v>
+      <c r="D77" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="B78" s="4"/>
-      <c r="C78" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>198</v>
+      <c r="C78" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="B80" s="4"/>
-      <c r="C80" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D80" s="10" t="s">
+      <c r="C80" s="4" t="s">
         <v>205</v>
       </c>
+      <c r="D80" s="14" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>206</v>
+      <c r="A81" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D81" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B82" s="4"/>
-      <c r="C82" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="C82" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B83" s="4"/>
-      <c r="C83" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>217</v>
+      <c r="C83" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>357</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>218</v>
+        <v>362</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>219</v>
+        <v>364</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>221</v>
+        <v>336</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>374</v>
+        <v>215</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="3" t="s">
-        <v>379</v>
+        <v>216</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="3" t="s">
-        <v>365</v>
+        <v>223</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>364</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>353</v>
+        <v>219</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>354</v>
+        <v>220</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="19" t="s">
         <v>227</v>
       </c>
       <c r="B91" s="4"/>
-      <c r="C91" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>231</v>
+      <c r="C91" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B92" s="4"/>
-      <c r="C92" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>230</v>
+      <c r="C92" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D93" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B93" s="4"/>
-      <c r="C93" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A94" s="19" t="s">
-        <v>236</v>
+    </row>
+    <row r="94" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>377</v>
       </c>
       <c r="B94" s="4"/>
-      <c r="C94" s="4" t="s">
-        <v>237</v>
+      <c r="C94" s="14" t="s">
+        <v>378</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>238</v>
+        <v>289</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B95" s="4"/>
+      <c r="C95" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D95" s="4" t="s">
+      <c r="D96" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
+      <c r="B97" s="4"/>
+      <c r="C97" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B96" s="4"/>
-      <c r="C96" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="D97" s="16" t="s">
-        <v>304</v>
+      <c r="D97" s="14" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>305</v>
+        <v>246</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>249</v>
+        <v>376</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>250</v>
+        <v>375</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>257</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B101" s="4"/>
-      <c r="C101" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>255</v>
+      <c r="C101" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A102" s="19" t="s">
+        <v>250</v>
       </c>
       <c r="B102" s="4"/>
-      <c r="C102" s="18" t="s">
-        <v>256</v>
+      <c r="C102" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>306</v>
+        <v>252</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="18" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B104" s="4"/>
-      <c r="C104" s="14" t="s">
+      <c r="D104" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D104" s="16" t="s">
+    </row>
+    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
         <v>262</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A105" s="19" t="s">
-        <v>265</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D105" s="16" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B106" s="4"/>
-      <c r="C106" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="D106" s="16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="B107" s="4"/>
-      <c r="C107" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>276</v>
+      <c r="C107" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>279</v>
+        <v>358</v>
+      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D108" s="25" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>280</v>
+      <c r="A109" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>314</v>
       </c>
       <c r="B110" s="4"/>
-      <c r="C110" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D111" s="25" t="s">
-        <v>377</v>
+      <c r="C110" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D111" s="24" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>284</v>
+      <c r="A112" s="4" t="s">
+        <v>319</v>
       </c>
       <c r="B112" s="4"/>
-      <c r="C112" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>302</v>
+      <c r="C112" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="14" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>334</v>
+        <v>270</v>
       </c>
       <c r="B114" s="4"/>
-      <c r="C114" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="D114" s="24" t="s">
-        <v>340</v>
+      <c r="C114" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>336</v>
+      <c r="A115" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="D115" s="16" t="s">
-        <v>341</v>
+        <v>279</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
-        <v>338</v>
+      <c r="A116" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="D116" s="16" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="B117" s="4"/>
-      <c r="C117" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="D117" s="16" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A117" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B117" s="20"/>
+      <c r="C117" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D117" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B118" s="4"/>
-      <c r="C118" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>292</v>
+        <v>299</v>
+      </c>
+      <c r="B118" s="20"/>
+      <c r="C118" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="D118" s="22" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B119" s="4"/>
-      <c r="C119" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A120" s="20" t="s">
-        <v>307</v>
+        <v>302</v>
+      </c>
+      <c r="B119" s="20"/>
+      <c r="C119" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="D119" s="22" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>305</v>
       </c>
       <c r="B120" s="20"/>
-      <c r="C120" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="D120" s="20" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="C120" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="D120" s="21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B121" s="20"/>
       <c r="C121" s="21" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D121" s="22" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B122" s="20"/>
-      <c r="C122" s="21" t="s">
-        <v>320</v>
+      <c r="A122" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C122" s="23" t="s">
+        <v>310</v>
       </c>
       <c r="D122" s="22" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B123" s="20"/>
-      <c r="C123" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C123" s="23" t="s">
+        <v>332</v>
+      </c>
+      <c r="D123" s="22" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="D123" s="21" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B124" s="20"/>
-      <c r="C124" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D124" s="22" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>327</v>
-      </c>
-      <c r="D125" s="22" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C126" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="D126" s="22" t="s">
-        <v>348</v>
+      <c r="B125" s="4"/>
+      <c r="C125" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B126" s="4"/>
+      <c r="C126" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="C127" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="D127" s="21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
+      <c r="A127" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="B127" s="26"/>
+      <c r="C127" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="A128" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="B128" s="26"/>
+      <c r="C128" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="B128" s="4"/>
-      <c r="C128" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B129" s="4"/>
-      <c r="C129" s="6" t="s">
+      <c r="D128" s="27" t="s">
         <v>371</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A130" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="B130" s="26"/>
-      <c r="C130" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D130" s="12" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A131" s="26" t="s">
-        <v>384</v>
-      </c>
-      <c r="B131" s="26"/>
-      <c r="C131" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="D131" s="27" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(CWL): add zone spawning helpers
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF246326-1F9B-41EC-93E4-458DA270196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6FE02B-8396-4853-9A41-5C932F6C7642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="2490" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13485" yWindow="4905" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="382">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3962,33 +3962,249 @@
   </si>
   <si>
     <r>
+      <t>&lt;color=blue&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标右键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/color&gt;</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_workbook_cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>workbook-cache: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_log_workbook_prefetch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>workbook-prefetch: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作簿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作簿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>缓存</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>): {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工作簿(预载)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>: {0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>詳細</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_ui_bgm_view</t>
+  </si>
+  <si>
+    <t>プレイリストを見る</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=#d343f7&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>MOD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与您当前游戏版本不兼容。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;/color&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+{0}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>&lt;color=purple&gt;&lt;[</t>
     </r>
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>マウスの左ボタン</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>詳細をコピー</t>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标左键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>复制详情</t>
     </r>
     <r>
       <rPr>
@@ -4002,11 +4218,50 @@
     <r>
       <rPr>
         <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>鼠标中键</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>关闭且不再显示</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;/color&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;color=purple&gt;&lt;[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
         <rFont val="Yu Gothic"/>
         <family val="3"/>
         <charset val="128"/>
       </rPr>
-      <t>マウスの中ボタン</t>
+      <t>マウスの左ボタン</t>
     </r>
     <r>
       <rPr>
@@ -4019,91 +4274,11 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="Yu Gothic"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>閉じて今後表示しない</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;/color&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=blue&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标右键</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关闭</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;/color&gt;</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=purple&gt;&lt;[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标左键</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>复制详情</t>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>詳細をコピー</t>
     </r>
     <r>
       <rPr>
@@ -4117,11 +4292,11 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>鼠标中键</t>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>マウスの中ボタン</t>
     </r>
     <r>
       <rPr>
@@ -4134,11 +4309,11 @@
     <r>
       <rPr>
         <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>关闭且不再显示</t>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>閉じて今後表示しない</t>
     </r>
     <r>
       <rPr>
@@ -4148,200 +4323,34 @@
       </rPr>
       <t>&gt;&lt;/color&gt;</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_log_workbook_cache</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>workbook-cache: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_log_workbook_prefetch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>workbook-prefetch: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>工作簿</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>: {0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>工作簿</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>缓存</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>): {0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>工作簿(预载)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color theme="1"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>: {0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重加载</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>详细</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>詳細</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_bgm_detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_ui_bgm_view</t>
-  </si>
-  <si>
-    <t>プレイリストを見る</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;color=#d343f7&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>一个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>MOD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>与您当前游戏版本不兼容。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;/color&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-{0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwl_warn_exist_zone</t>
+  </si>
+  <si>
+    <t>failed to create zone: {0}
+A zone already exists at {1}, {2}: {3}</t>
+  </si>
+  <si>
+    <t>取消生成区域: {0}
+一个区域已经存在于 {1}, {2}: {3}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4399,7 +4408,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -4506,13 +4515,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="15.8"/>
-      <color theme="1"/>
-      <name val="Cascadia Code"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4608,8 +4610,8 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4891,22 +4893,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="52.375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="93.75" style="9" customWidth="1"/>
-    <col min="4" max="4" width="156.125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="93.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="156.140625" style="7" customWidth="1"/>
     <col min="5" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4920,7 +4922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="23.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -4934,13 +4936,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="23.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="23.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -4952,7 +4954,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="23.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -4964,7 +4966,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="46.5">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -4976,7 +4978,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="23.25">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -4988,7 +4990,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="46.5">
       <c r="A8" s="5" t="s">
         <v>43</v>
       </c>
@@ -5000,7 +5002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="46.5">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -5012,7 +5014,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="23.25">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -5023,7 +5025,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="23.25">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -5035,7 +5037,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="23.25">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -5047,7 +5049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="23.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -5059,7 +5061,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="9" customFormat="1" ht="23.25">
       <c r="A14" s="4" t="s">
         <v>126</v>
       </c>
@@ -5071,7 +5073,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="23.25">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
@@ -5083,7 +5085,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="23.25">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="23.25">
       <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
@@ -5107,7 +5109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="23.25">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -5119,7 +5121,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="23.25">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -5131,7 +5133,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="23.25">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="46.5">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
@@ -5155,7 +5157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="23.25">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
@@ -5166,7 +5168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="23.25">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -5177,7 +5179,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="23.25">
       <c r="A24" s="4" t="s">
         <v>123</v>
       </c>
@@ -5189,7 +5191,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" s="9" customFormat="1" ht="23.25">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -5201,7 +5203,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="23.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -5213,7 +5215,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="23.25">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
@@ -5225,7 +5227,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="23.25">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
@@ -5234,10 +5236,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.25">
       <c r="A29" s="4" t="s">
         <v>55</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="23.25">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -5261,7 +5263,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="23.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -5273,7 +5275,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="23.25">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
@@ -5285,7 +5287,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="23.25">
       <c r="A33" s="4" t="s">
         <v>29</v>
       </c>
@@ -5297,7 +5299,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="23.25">
       <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
@@ -5309,7 +5311,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="23.25">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
@@ -5321,7 +5323,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="46.5">
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
@@ -5333,7 +5335,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="46.5">
       <c r="A37" s="4" t="s">
         <v>28</v>
       </c>
@@ -5345,7 +5347,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="69.75">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -5357,7 +5359,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="93" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="93">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -5369,7 +5371,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="69.75">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -5381,7 +5383,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="46.5">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -5393,7 +5395,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="46.5">
       <c r="A42" s="2" t="s">
         <v>65</v>
       </c>
@@ -5405,7 +5407,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="46.5">
       <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
@@ -5417,7 +5419,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="23.25">
       <c r="A44" s="4" t="s">
         <v>127</v>
       </c>
@@ -5429,7 +5431,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="23.25">
       <c r="A45" s="5" t="s">
         <v>128</v>
       </c>
@@ -5441,7 +5443,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="93" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="93">
       <c r="A46" s="2" t="s">
         <v>122</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="46.5">
       <c r="A47" s="2" t="s">
         <v>129</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" s="8" customFormat="1" ht="23.25">
       <c r="A48" s="13" t="s">
         <v>130</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="8" customFormat="1" ht="186" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" s="8" customFormat="1" ht="209.25">
       <c r="A49" s="13" t="s">
         <v>131</v>
       </c>
@@ -5485,7 +5487,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="46.5">
       <c r="A50" s="2" t="s">
         <v>73</v>
       </c>
@@ -5496,7 +5498,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="23.25">
       <c r="A51" s="2" t="s">
         <v>75</v>
       </c>
@@ -5507,7 +5509,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="23.25">
       <c r="A52" s="4" t="s">
         <v>167</v>
       </c>
@@ -5519,7 +5521,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="23.25">
       <c r="A53" s="4" t="s">
         <v>104</v>
       </c>
@@ -5531,7 +5533,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="46.5">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -5543,7 +5545,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="23.25">
       <c r="A55" s="4" t="s">
         <v>121</v>
       </c>
@@ -5555,7 +5557,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="116.25">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -5567,7 +5569,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="69.75">
       <c r="A57" s="2" t="s">
         <v>113</v>
       </c>
@@ -5579,7 +5581,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="23.25">
       <c r="A58" s="4" t="s">
         <v>115</v>
       </c>
@@ -5591,7 +5593,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="46.5">
       <c r="A59" s="4" t="s">
         <v>118</v>
       </c>
@@ -5603,7 +5605,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="23.25">
       <c r="A60" s="2" t="s">
         <v>120</v>
       </c>
@@ -5615,7 +5617,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="46.5">
       <c r="A61" s="2" t="s">
         <v>157</v>
       </c>
@@ -5626,7 +5628,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="23.25">
       <c r="A62" s="2" t="s">
         <v>158</v>
       </c>
@@ -5637,7 +5639,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="23.25">
       <c r="A63" s="2" t="s">
         <v>159</v>
       </c>
@@ -5648,7 +5650,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="23.25">
       <c r="A64" s="4" t="s">
         <v>295</v>
       </c>
@@ -5660,7 +5662,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="23.25">
       <c r="A65" s="4" t="s">
         <v>296</v>
       </c>
@@ -5672,7 +5674,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="23.25">
       <c r="A66" s="4" t="s">
         <v>166</v>
       </c>
@@ -5684,7 +5686,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="46.5">
       <c r="A67" s="4" t="s">
         <v>170</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="23.25">
       <c r="A68" s="4" t="s">
         <v>172</v>
       </c>
@@ -5708,7 +5710,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="23.25">
       <c r="A69" s="4" t="s">
         <v>173</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="46.5">
       <c r="A70" s="2" t="s">
         <v>174</v>
       </c>
@@ -5732,7 +5734,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="23.25">
       <c r="A71" s="4" t="s">
         <v>175</v>
       </c>
@@ -5744,7 +5746,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="23.25">
       <c r="A72" s="5" t="s">
         <v>179</v>
       </c>
@@ -5756,7 +5758,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="46.5">
       <c r="A73" s="5" t="s">
         <v>183</v>
       </c>
@@ -5768,7 +5770,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="23.25">
       <c r="A74" s="5" t="s">
         <v>180</v>
       </c>
@@ -5780,7 +5782,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="23.25">
       <c r="A75" s="2" t="s">
         <v>186</v>
       </c>
@@ -5792,7 +5794,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="23.25">
       <c r="A76" s="4" t="s">
         <v>188</v>
       </c>
@@ -5804,7 +5806,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="46.5">
       <c r="A77" s="2" t="s">
         <v>195</v>
       </c>
@@ -5816,7 +5818,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="46.5">
       <c r="A78" s="2" t="s">
         <v>198</v>
       </c>
@@ -5828,7 +5830,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="23.25">
       <c r="A79" s="4" t="s">
         <v>203</v>
       </c>
@@ -5840,7 +5842,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="23.25">
       <c r="A80" s="4" t="s">
         <v>204</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="46.5">
       <c r="A81" s="5" t="s">
         <v>209</v>
       </c>
@@ -5864,7 +5866,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="25.5">
       <c r="A82" s="4" t="s">
         <v>212</v>
       </c>
@@ -5876,7 +5878,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="25.5">
       <c r="A83" s="4" t="s">
         <v>213</v>
       </c>
@@ -5885,22 +5887,22 @@
         <v>360</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="51" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="51">
       <c r="A84" s="4" t="s">
         <v>356</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>361</v>
+        <v>378</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="25.5">
       <c r="A85" s="4" t="s">
         <v>214</v>
       </c>
@@ -5912,7 +5914,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="23.25">
       <c r="A86" s="4" t="s">
         <v>335</v>
       </c>
@@ -5924,7 +5926,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="23.25">
       <c r="A87" s="4" t="s">
         <v>215</v>
       </c>
@@ -5936,7 +5938,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="23.25">
       <c r="A88" s="4" t="s">
         <v>218</v>
       </c>
@@ -5948,7 +5950,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="23.25">
       <c r="A89" s="4" t="s">
         <v>219</v>
       </c>
@@ -5960,7 +5962,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="23.25">
       <c r="A90" s="4" t="s">
         <v>224</v>
       </c>
@@ -5972,7 +5974,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="23.25">
       <c r="A91" s="19" t="s">
         <v>227</v>
       </c>
@@ -5984,7 +5986,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="23.25">
       <c r="A92" s="4" t="s">
         <v>230</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="23.25">
       <c r="A93" s="4" t="s">
         <v>232</v>
       </c>
@@ -6008,19 +6010,19 @@
         <v>233</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" s="9" customFormat="1" ht="23.25">
       <c r="A94" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="23.25">
       <c r="A95" s="4" t="s">
         <v>236</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="25.5">
       <c r="A96" s="4" t="s">
         <v>238</v>
       </c>
@@ -6044,7 +6046,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="23.25">
       <c r="A97" s="4" t="s">
         <v>240</v>
       </c>
@@ -6053,10 +6055,10 @@
         <v>241</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="25.5">
       <c r="A98" s="4" t="s">
         <v>242</v>
       </c>
@@ -6065,22 +6067,22 @@
         <v>246</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="23.25">
       <c r="A99" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="25.5">
       <c r="A100" s="4" t="s">
         <v>254</v>
       </c>
@@ -6092,7 +6094,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="23.25">
       <c r="A101" s="4" t="s">
         <v>245</v>
       </c>
@@ -6104,7 +6106,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="23.25">
       <c r="A102" s="19" t="s">
         <v>250</v>
       </c>
@@ -6116,7 +6118,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="25.5">
       <c r="A103" s="4" t="s">
         <v>253</v>
       </c>
@@ -6128,7 +6130,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="23.25">
       <c r="A104" s="4" t="s">
         <v>259</v>
       </c>
@@ -6140,7 +6142,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="23.25">
       <c r="A105" s="2" t="s">
         <v>262</v>
       </c>
@@ -6152,7 +6154,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="23.25">
       <c r="A106" s="4" t="s">
         <v>265</v>
       </c>
@@ -6164,7 +6166,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="69.75">
       <c r="A107" s="2" t="s">
         <v>266</v>
       </c>
@@ -6176,7 +6178,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="23.25">
       <c r="A108" s="2" t="s">
         <v>357</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="23.25">
       <c r="A109" s="2" t="s">
         <v>269</v>
       </c>
@@ -6200,7 +6202,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="23.25">
       <c r="A110" s="4" t="s">
         <v>314</v>
       </c>
@@ -6212,7 +6214,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="45">
       <c r="A111" s="4" t="s">
         <v>317</v>
       </c>
@@ -6224,7 +6226,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="23.25">
       <c r="A112" s="4" t="s">
         <v>319</v>
       </c>
@@ -6236,7 +6238,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="23.25">
       <c r="A113" s="4" t="s">
         <v>321</v>
       </c>
@@ -6248,7 +6250,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="25.5">
       <c r="A114" s="4" t="s">
         <v>270</v>
       </c>
@@ -6260,7 +6262,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="23.25">
       <c r="A115" s="2" t="s">
         <v>275</v>
       </c>
@@ -6272,7 +6274,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="23.25">
       <c r="A116" s="2" t="s">
         <v>276</v>
       </c>
@@ -6284,7 +6286,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="23.25">
       <c r="A117" s="20" t="s">
         <v>290</v>
       </c>
@@ -6296,7 +6298,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="46.5">
       <c r="A118" s="2" t="s">
         <v>299</v>
       </c>
@@ -6308,7 +6310,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="23.25">
       <c r="A119" s="2" t="s">
         <v>302</v>
       </c>
@@ -6320,7 +6322,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="69.75" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="69.75">
       <c r="A120" s="2" t="s">
         <v>305</v>
       </c>
@@ -6329,10 +6331,10 @@
         <v>333</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="45.75" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="45.75">
       <c r="A121" s="2" t="s">
         <v>306</v>
       </c>
@@ -6344,7 +6346,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="46.5">
       <c r="A122" s="4" t="s">
         <v>309</v>
       </c>
@@ -6355,7 +6357,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="23.25">
       <c r="A123" s="2" t="s">
         <v>330</v>
       </c>
@@ -6366,7 +6368,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="23.25">
       <c r="A124" s="4" t="s">
         <v>337</v>
       </c>
@@ -6377,7 +6379,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="69">
       <c r="A125" s="4" t="s">
         <v>350</v>
       </c>
@@ -6389,7 +6391,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="46.5">
       <c r="A126" s="4" t="s">
         <v>351</v>
       </c>
@@ -6401,29 +6403,71 @@
         <v>354</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="23.25">
       <c r="A127" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="B127" s="26"/>
+      <c r="C127" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="D127" s="26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="23.25">
+      <c r="A128" s="26" t="s">
         <v>364</v>
-      </c>
-      <c r="B127" s="26"/>
-      <c r="C127" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="D127" s="12" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="A128" s="26" t="s">
-        <v>366</v>
       </c>
       <c r="B128" s="26"/>
       <c r="C128" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="D128" s="27" t="s">
-        <v>370</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="D128" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="46.5">
+      <c r="A129" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B129" s="26"/>
+      <c r="C129" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="D129" s="27" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="23.25">
+      <c r="A130" s="26"/>
+      <c r="B130" s="26"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="26"/>
+    </row>
+    <row r="131" spans="1:4" ht="23.25">
+      <c r="A131" s="26"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="26"/>
+      <c r="D131" s="26"/>
+    </row>
+    <row r="132" spans="1:4" ht="23.25">
+      <c r="A132" s="26"/>
+      <c r="B132" s="26"/>
+      <c r="C132" s="26"/>
+      <c r="D132" s="26"/>
+    </row>
+    <row r="133" spans="1:4" ht="23.25">
+      <c r="A133" s="26"/>
+      <c r="B133" s="26"/>
+      <c r="C133" s="26"/>
+      <c r="D133" s="26"/>
+    </row>
+    <row r="134" spans="1:4" ht="23.25">
+      <c r="A134" s="26"/>
+      <c r="B134" s="26"/>
+      <c r="C134" s="26"/>
+      <c r="D134" s="26"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): console pipe server
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6FE02B-8396-4853-9A41-5C932F6C7642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71922BCC-78B4-43DD-BF25-3E62E9A74D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13485" yWindow="4905" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="3990" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="385">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2381,72 +2381,6 @@
   </si>
   <si>
     <t>ひよこの掃除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_warn_fix_actCombat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwl_warn_fix_listAbility</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>角色 {1} 移除了无效的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> actCombat ID: {0}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色 {1} 移除了无效的 listAbility ID: {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">removed invalid actCombat ID: {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>from {1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">removed invalid listAbility ID: {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>from {1}</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2971,80 +2905,6 @@
   </si>
   <si>
     <r>
-      <t>エラーが発生した時点でのアプリの動作</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>最も新しいものが一番上です</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>):</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>导致此错误的事件顺序</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>最后的事件在最上方</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>):</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="15.8"/>
         <rFont val="宋体"/>
@@ -3254,61 +3114,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>已将角色</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> {1} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="微软雅黑"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的无效</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cascadia Code"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Hobby {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>移除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>キャラクター {1} の無効なHobby {0} を削除しました</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>&lt;color=#d343f7&gt;MOD</t>
     </r>
     <r>
@@ -4334,13 +4139,158 @@
   <si>
     <t>取消生成区域: {0}
 一个区域已经存在于 {1}, {2}: {3}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>//导致此错误的事件顺序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最后的事件在最上方</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>//エラーが発生した時点でのアプリの動作</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最も新しいものが一番上です</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <t>cwl_ui_debug_btn</t>
+  </si>
+  <si>
+    <t>CWL/デバッグをオンにする</t>
+  </si>
+  <si>
+    <t>CWL/启用调试</t>
+  </si>
+  <si>
+    <t>cwl_warn_fix_actCombat</t>
+  </si>
+  <si>
+    <t>無効なactCombat '&lt;color=red&gt;{0}&lt;/color&gt;' を '{1}' から削除しました</t>
+  </si>
+  <si>
+    <t>cwl_warn_fix_listAbility</t>
+  </si>
+  <si>
+    <t>無効なlistAbility '&lt;color=red&gt;{0}&lt;/color&gt;' を '{1}' から削除しました</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">已从 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>'{1}' 移除无效的actCombat '&lt;color=red&gt;{0}&lt;/color&gt;'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">已从 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>'{1}' 移除无效的listAbility '&lt;color=red&gt;{0}&lt;/color&gt;'</t>
+    </r>
+  </si>
+  <si>
+    <t>無効なHobby '&lt;color=red&gt;{0}&lt;/color&gt;' を '{1}' から削除しました</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">已从 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Cascadia Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>'{1}' 移除无效的Hobby '&lt;color=red&gt;{0}&lt;/color&gt;'</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4515,6 +4465,18 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4536,7 +4498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4595,12 +4557,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4611,6 +4567,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4895,15 +4854,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="52.42578125" style="9" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="93.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="109.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="156.140625" style="7" customWidth="1"/>
     <col min="5" max="16384" width="9" style="7"/>
   </cols>
@@ -4972,10 +4931,10 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25">
@@ -5236,7 +5195,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25">
@@ -5371,7 +5330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="69.75">
+    <row r="40" spans="1:4" ht="46.5">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -5389,10 +5348,10 @@
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="3" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="46.5">
@@ -5448,10 +5407,10 @@
         <v>122</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="46.5">
@@ -5476,15 +5435,15 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="8" customFormat="1" ht="209.25">
+    <row r="49" spans="1:4" s="8" customFormat="1" ht="186">
       <c r="A49" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="46.5">
@@ -5557,7 +5516,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="116.25">
+    <row r="56" spans="1:4" ht="69.75">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -5611,10 +5570,10 @@
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="46.5">
@@ -5652,26 +5611,26 @@
     </row>
     <row r="64" spans="1:4" ht="23.25">
       <c r="A64" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25">
       <c r="A65" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25">
@@ -5680,10 +5639,10 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="14" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="46.5">
@@ -5692,10 +5651,10 @@
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25">
@@ -5872,10 +5831,10 @@
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="25.5">
@@ -5884,22 +5843,22 @@
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="51">
       <c r="A84" s="4" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="25.5">
@@ -5908,22 +5867,22 @@
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="23.25">
       <c r="A86" s="4" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="3" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="23.25">
@@ -6012,14 +5971,14 @@
     </row>
     <row r="94" spans="1:4" s="9" customFormat="1" ht="23.25">
       <c r="A94" s="4" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="14" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="23.25">
@@ -6055,7 +6014,7 @@
         <v>241</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5">
@@ -6067,19 +6026,19 @@
         <v>246</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25">
       <c r="A99" s="4" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5">
@@ -6160,10 +6119,10 @@
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="69.75">
@@ -6172,22 +6131,22 @@
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="23.25">
       <c r="A108" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D108" s="25" t="s">
-        <v>359</v>
+        <v>348</v>
+      </c>
+      <c r="D108" s="23" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25">
@@ -6196,278 +6155,284 @@
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="23.25">
       <c r="A110" s="4" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="14" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="45">
       <c r="A111" s="4" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="D111" s="24" t="s">
-        <v>323</v>
+        <v>310</v>
+      </c>
+      <c r="D111" s="22" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="23.25">
       <c r="A112" s="4" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B112" s="4"/>
-      <c r="C112" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>324</v>
+      <c r="C112" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D112" s="21" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="23.25">
       <c r="A113" s="4" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B113" s="4"/>
-      <c r="C113" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="D113" s="16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="25.5">
+      <c r="C113" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="23.25">
       <c r="A114" s="4" t="s">
         <v>270</v>
       </c>
       <c r="B114" s="4"/>
-      <c r="C114" s="18" t="s">
+      <c r="C114" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="D114" s="16" t="s">
+      <c r="D114" s="21" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="23.25">
+    <row r="115" spans="1:4" ht="46.5">
       <c r="A115" s="2" t="s">
-        <v>275</v>
+        <v>377</v>
       </c>
       <c r="B115" s="4"/>
-      <c r="C115" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="23.25">
+      <c r="C115" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="D115" s="26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="46.5">
       <c r="A116" s="2" t="s">
-        <v>276</v>
+        <v>379</v>
       </c>
       <c r="B116" s="4"/>
-      <c r="C116" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>278</v>
+      <c r="C116" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="23.25">
       <c r="A117" s="20" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B117" s="20"/>
-      <c r="C117" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="D117" s="20" t="s">
-        <v>292</v>
+      <c r="C117" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="46.5">
       <c r="A118" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B118" s="20"/>
       <c r="C118" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="D118" s="22" t="s">
-        <v>301</v>
+        <v>294</v>
+      </c>
+      <c r="D118" s="21" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="23.25">
       <c r="A119" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B119" s="20"/>
       <c r="C119" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="D119" s="22" t="s">
-        <v>304</v>
+        <v>297</v>
+      </c>
+      <c r="D119" s="21" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="69.75">
       <c r="A120" s="2" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B120" s="20"/>
       <c r="C120" s="21" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="45.75">
       <c r="A121" s="2" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B121" s="20"/>
       <c r="C121" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="D121" s="22" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="46.5">
+        <v>301</v>
+      </c>
+      <c r="D121" s="21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="23.25">
       <c r="A122" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C122" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="D122" s="22" t="s">
-        <v>311</v>
+        <v>303</v>
+      </c>
+      <c r="C122" s="21" t="s">
+        <v>373</v>
+      </c>
+      <c r="D122" s="21" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="23.25">
       <c r="A123" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C123" s="23" t="s">
-        <v>332</v>
-      </c>
-      <c r="D123" s="22" t="s">
-        <v>331</v>
+        <v>322</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="D123" s="26" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="23.25">
       <c r="A124" s="4" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D124" s="21" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="69">
       <c r="A125" s="4" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="6" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="46.5">
       <c r="A126" s="4" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="23.25">
+      <c r="A127" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B127" s="24"/>
+      <c r="C127" s="24" t="s">
         <v>353</v>
       </c>
-      <c r="D126" s="6" t="s">
+      <c r="D127" s="24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="23.25">
+      <c r="A128" s="24" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="23.25">
-      <c r="A127" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="B127" s="26"/>
-      <c r="C127" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="D127" s="26" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="23.25">
-      <c r="A128" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="B128" s="26"/>
-      <c r="C128" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="D128" s="26" t="s">
-        <v>368</v>
+      <c r="B128" s="24"/>
+      <c r="C128" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="D128" s="24" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="46.5">
       <c r="A129" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="B129" s="26"/>
-      <c r="C129" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="D129" s="27" t="s">
-        <v>381</v>
+        <v>369</v>
+      </c>
+      <c r="B129" s="24"/>
+      <c r="C129" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="D129" s="25" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="23.25">
-      <c r="A130" s="26"/>
-      <c r="B130" s="26"/>
-      <c r="C130" s="26"/>
-      <c r="D130" s="26"/>
+      <c r="A130" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="B130" s="20"/>
+      <c r="C130" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="D130" s="20" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="131" spans="1:4" ht="23.25">
-      <c r="A131" s="26"/>
-      <c r="B131" s="26"/>
-      <c r="C131" s="26"/>
-      <c r="D131" s="26"/>
+      <c r="A131" s="24"/>
+      <c r="B131" s="24"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="24"/>
     </row>
     <row r="132" spans="1:4" ht="23.25">
-      <c r="A132" s="26"/>
-      <c r="B132" s="26"/>
-      <c r="C132" s="26"/>
-      <c r="D132" s="26"/>
+      <c r="A132" s="24"/>
+      <c r="B132" s="24"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="24"/>
     </row>
     <row r="133" spans="1:4" ht="23.25">
-      <c r="A133" s="26"/>
-      <c r="B133" s="26"/>
-      <c r="C133" s="26"/>
-      <c r="D133" s="26"/>
+      <c r="A133" s="24"/>
+      <c r="B133" s="24"/>
+      <c r="C133" s="24"/>
+      <c r="D133" s="24"/>
     </row>
     <row r="134" spans="1:4" ht="23.25">
-      <c r="A134" s="26"/>
-      <c r="B134" s="26"/>
-      <c r="C134" s="26"/>
-      <c r="D134" s="26"/>
+      <c r="A134" s="24"/>
+      <c r="B134" s="24"/>
+      <c r="C134" s="24"/>
+      <c r="D134" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>

<commit_message>
feat(CWL): allow custom zone asset loading
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62EB1F2-57E1-4140-BDD1-B05A0467BCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46978744-AE6E-457B-9C07-6A40967E6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13635" yWindow="3495" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15810" yWindow="4200" windowWidth="25710" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="391">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4284,6 +4284,26 @@
       </rPr>
       <t>'{2}' 移除无效的 {0} '&lt;color=red&gt;{1}&lt;/color&gt;'</t>
     </r>
+  </si>
+  <si>
+    <t>cwl_ui_export_zone</t>
+  </si>
+  <si>
+    <t>CWL/ゾーンを書き出す</t>
+  </si>
+  <si>
+    <t>cwl_relocate_zone</t>
+  </si>
+  <si>
+    <t>relocated zone &gt; {0}:{1}
+&gt; {2}</t>
+  </si>
+  <si>
+    <t>CWL/导出地图</t>
+  </si>
+  <si>
+    <t>重定向地图 &gt; {0}:{1}
+&gt; {2}</t>
   </si>
 </sst>
 </file>
@@ -4854,8 +4874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="C117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -6411,16 +6431,28 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="23.25">
-      <c r="A131" s="24"/>
+      <c r="A131" s="24" t="s">
+        <v>385</v>
+      </c>
       <c r="B131" s="24"/>
-      <c r="C131" s="24"/>
-      <c r="D131" s="24"/>
-    </row>
-    <row r="132" spans="1:4" ht="23.25">
-      <c r="A132" s="24"/>
+      <c r="C131" s="24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D131" s="24" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="46.5">
+      <c r="A132" s="24" t="s">
+        <v>387</v>
+      </c>
       <c r="B132" s="24"/>
-      <c r="C132" s="24"/>
-      <c r="D132" s="24"/>
+      <c r="C132" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="D132" s="25" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="133" spans="1:4" ht="23.25">
       <c r="A133" s="24"/>

</xml_diff>

<commit_message>
fix(CWL): drama `choice()` action and better exception handling
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46978744-AE6E-457B-9C07-6A40967E6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10CB5AF-7985-4881-832B-B15655E06746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="4200" windowWidth="25710" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="4470" windowWidth="25710" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -3314,30 +3314,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>正在使用 CWL &lt;color=#21a366&gt;稳定版&lt;/color&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>正在使用 CWL &lt;color=#427ddc&gt;Nightly&lt;/color&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[CWL] {0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15.8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>正在后台处理数据
-{1}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">[CWL] {0} </t>
     </r>
@@ -4304,6 +4280,27 @@
   <si>
     <t>重定向地图 &gt; {0}:{1}
 &gt; {2}</t>
+  </si>
+  <si>
+    <t>正在使用 CWL &lt;color=#427ddc&gt;夜间版 Nightly&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>正在使用 CWL &lt;color=#21a366&gt;稳定版 Stable&lt;/color&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[CWL] {0} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15.8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>正在处理数据
+{1}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4874,8 +4871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -5215,7 +5212,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="23.25">
@@ -5638,7 +5635,7 @@
         <v>291</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>332</v>
+        <v>389</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="23.25">
@@ -5650,7 +5647,7 @@
         <v>292</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>333</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="23.25">
@@ -5671,10 +5668,10 @@
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>334</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="23.25">
@@ -5851,10 +5848,10 @@
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="25.5">
@@ -5863,22 +5860,22 @@
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="51">
       <c r="A84" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="25.5">
@@ -5887,10 +5884,10 @@
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="23.25">
@@ -5991,11 +5988,11 @@
     </row>
     <row r="94" spans="1:4" s="9" customFormat="1" ht="23.25">
       <c r="A94" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>283</v>
@@ -6034,7 +6031,7 @@
         <v>241</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="25.5">
@@ -6046,19 +6043,19 @@
         <v>246</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="23.25">
       <c r="A99" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="16" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="25.5">
@@ -6159,14 +6156,14 @@
     </row>
     <row r="108" spans="1:4" ht="23.25">
       <c r="A108" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="23.25">
@@ -6243,26 +6240,26 @@
     </row>
     <row r="115" spans="1:4" ht="46.5">
       <c r="A115" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="D115" s="26" t="s">
         <v>378</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="46.5">
       <c r="A116" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="21" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="23.25">
@@ -6310,7 +6307,7 @@
         <v>323</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="45.75">
@@ -6330,10 +6327,10 @@
         <v>303</v>
       </c>
       <c r="C122" s="21" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="23.25">
@@ -6341,10 +6338,10 @@
         <v>322</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="23.25">
@@ -6360,98 +6357,98 @@
     </row>
     <row r="125" spans="1:4" ht="69">
       <c r="A125" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D125" s="6" t="s">
         <v>342</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="46.5">
       <c r="A126" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="23.25">
       <c r="A127" s="24" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B127" s="24"/>
       <c r="C127" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D127" s="24" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="23.25">
       <c r="A128" s="24" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B128" s="24"/>
       <c r="C128" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="D128" s="24" t="s">
         <v>355</v>
-      </c>
-      <c r="D128" s="24" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="46.5">
       <c r="A129" s="19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B129" s="24"/>
       <c r="C129" s="25" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D129" s="25" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="23.25">
       <c r="A130" s="20" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B130" s="20"/>
       <c r="C130" s="20" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="23.25">
       <c r="A131" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B131" s="24"/>
       <c r="C131" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D131" s="24" t="s">
         <v>386</v>
-      </c>
-      <c r="D131" s="24" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="46.5">
       <c r="A132" s="24" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B132" s="24"/>
       <c r="C132" s="25" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D132" s="25" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="23.25">

</xml_diff>

<commit_message>
feat(CWL): complete csharp eval & compiler support
</commit_message>
<xml_diff>
--- a/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
+++ b/CustomWhateverLoader/LangMod/CN/cwl_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CustomWhateverLoader\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10CB5AF-7985-4881-832B-B15655E06746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5910A226-6FCA-4184-B89F-8F4313704AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="4470" windowWidth="25710" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="735" windowWidth="30045" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="415">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4301,13 +4301,91 @@
       <t>正在处理数据
 {1}</t>
     </r>
+  </si>
+  <si>
+    <t>cwl_log_csc_roslyn</t>
+  </si>
+  <si>
+    <t>Roslyn コンパイラを使用しています {0}</t>
+  </si>
+  <si>
+    <t>cwl_log_csc_package</t>
+  </si>
+  <si>
+    <t>{1} からパッケージ {0} をコンパイルしています</t>
+  </si>
+  <si>
+    <t>cwl_log_csc_eval</t>
+  </si>
+  <si>
+    <t>スクリプトをコンパイルしています
+{0}</t>
+  </si>
+  <si>
+    <t>cwl_error_cs_disabled</t>
+  </si>
+  <si>
+    <t>スクリプトコンパイラは無効化されています</t>
+  </si>
+  <si>
+    <t>cwl_log_csc_scripts</t>
+  </si>
+  <si>
+    <t>cwl_error_csc_diag</t>
+  </si>
+  <si>
+    <t>「{0}」のコンパイルに失敗しました:
+{1}</t>
+  </si>
+  <si>
+    <t>cwl_error_cs_frozen</t>
+  </si>
+  <si>
+    <t>スクリプト状態「{0}」は凍結されています</t>
+  </si>
+  <si>
+    <t>Roslyn 编译器 {0}</t>
+  </si>
+  <si>
+    <t>正在编译脚本
+{0}</t>
+  </si>
+  <si>
+    <t>脚本编译器已被禁用</t>
+  </si>
+  <si>
+    <t>编译 '{0}' 失败:
+{1}</t>
+  </si>
+  <si>
+    <t>脚本状态 '{0}' 已被冻结</t>
+  </si>
+  <si>
+    <t>正在编译 {1} 个脚本文件 '{0}'</t>
+  </si>
+  <si>
+    <t>{1} 個のスクリプトファイルをコンパイルしています '{0}'</t>
+  </si>
+  <si>
+    <t>正在编译包 {0} &lt;&lt; {1}</t>
+  </si>
+  <si>
+    <t>cwl_warn_drama_call_ex</t>
+  </si>
+  <si>
+    <t>call failure: '{0}'
+{1}</t>
+  </si>
+  <si>
+    <t>调用失败: '{0}'
+{1}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4494,6 +4572,12 @@
       <name val="Cascadia Code"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="15.8"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4515,7 +4599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4588,6 +4672,9 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4869,16 +4956,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D134"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="7" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="109.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="156.140625" style="7" customWidth="1"/>
     <col min="5" max="16384" width="9" style="7"/>
@@ -6403,27 +6490,27 @@
         <v>355</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="46.5">
-      <c r="A129" s="19" t="s">
+    <row r="129" spans="1:4" ht="23.25">
+      <c r="A129" s="24" t="s">
         <v>366</v>
       </c>
       <c r="B129" s="24"/>
-      <c r="C129" s="25" t="s">
+      <c r="C129" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="D129" s="25" t="s">
+      <c r="D129" s="24" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="23.25">
-      <c r="A130" s="20" t="s">
+      <c r="A130" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="B130" s="20"/>
-      <c r="C130" s="20" t="s">
+      <c r="B130" s="24"/>
+      <c r="C130" s="24" t="s">
         <v>372</v>
       </c>
-      <c r="D130" s="20" t="s">
+      <c r="D130" s="24" t="s">
         <v>373</v>
       </c>
     </row>
@@ -6439,29 +6526,191 @@
         <v>386</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="46.5">
+    <row r="132" spans="1:4" ht="23.25">
       <c r="A132" s="24" t="s">
         <v>384</v>
       </c>
       <c r="B132" s="24"/>
-      <c r="C132" s="25" t="s">
+      <c r="C132" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="D132" s="25" t="s">
+      <c r="D132" s="24" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="23.25">
-      <c r="A133" s="24"/>
+      <c r="A133" s="24" t="s">
+        <v>391</v>
+      </c>
       <c r="B133" s="24"/>
-      <c r="C133" s="24"/>
-      <c r="D133" s="24"/>
+      <c r="C133" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="D133" s="24" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="134" spans="1:4" ht="23.25">
-      <c r="A134" s="24"/>
+      <c r="A134" s="24" t="s">
+        <v>393</v>
+      </c>
       <c r="B134" s="24"/>
-      <c r="C134" s="24"/>
-      <c r="D134" s="24"/>
+      <c r="C134" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="D134" s="24" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="46.5">
+      <c r="A135" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="B135" s="24"/>
+      <c r="C135" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="D135" s="25" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="23.25">
+      <c r="A136" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B136" s="24"/>
+      <c r="C136" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="D136" s="24" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="23.25">
+      <c r="A137" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="B137" s="24"/>
+      <c r="C137" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="D137" s="24" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="46.5">
+      <c r="A138" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B138" s="24"/>
+      <c r="C138" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="D138" s="25" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="23.25">
+      <c r="A139" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="D139" s="24" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="46.5">
+      <c r="A140" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="B140" s="24"/>
+      <c r="C140" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="D140" s="25" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="23.25">
+      <c r="A141" s="24"/>
+      <c r="B141" s="24"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+    </row>
+    <row r="142" spans="1:4" ht="23.25">
+      <c r="A142" s="24"/>
+      <c r="B142" s="24"/>
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+    </row>
+    <row r="143" spans="1:4" ht="23.25">
+      <c r="A143" s="24"/>
+      <c r="B143" s="24"/>
+      <c r="C143" s="24"/>
+      <c r="D143" s="24"/>
+    </row>
+    <row r="144" spans="1:4" ht="23.25">
+      <c r="A144" s="24"/>
+      <c r="B144" s="24"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+    </row>
+    <row r="145" spans="1:4" ht="23.25">
+      <c r="A145" s="24"/>
+      <c r="B145" s="24"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+    </row>
+    <row r="146" spans="1:4" ht="23.25">
+      <c r="A146" s="24"/>
+      <c r="B146" s="24"/>
+      <c r="C146" s="24"/>
+      <c r="D146" s="24"/>
+    </row>
+    <row r="147" spans="1:4" ht="23.25">
+      <c r="A147" s="24"/>
+      <c r="B147" s="24"/>
+      <c r="C147" s="24"/>
+      <c r="D147" s="24"/>
+    </row>
+    <row r="148" spans="1:4" ht="23.25">
+      <c r="A148" s="24"/>
+      <c r="B148" s="24"/>
+      <c r="C148" s="24"/>
+      <c r="D148" s="24"/>
+    </row>
+    <row r="149" spans="1:4" ht="23.25">
+      <c r="A149" s="24"/>
+      <c r="B149" s="24"/>
+      <c r="C149" s="24"/>
+      <c r="D149" s="24"/>
+    </row>
+    <row r="150" spans="1:4" ht="23.25">
+      <c r="A150" s="24"/>
+      <c r="B150" s="24"/>
+      <c r="C150" s="24"/>
+      <c r="D150" s="24"/>
+    </row>
+    <row r="151" spans="1:4" ht="23.25">
+      <c r="A151" s="24"/>
+      <c r="B151" s="24"/>
+      <c r="C151" s="24"/>
+      <c r="D151" s="24"/>
+    </row>
+    <row r="152" spans="1:4" ht="23.25">
+      <c r="A152" s="24"/>
+      <c r="B152" s="24"/>
+      <c r="C152" s="24"/>
+      <c r="D152" s="24"/>
+    </row>
+    <row r="153" spans="1:4" ht="23.25">
+      <c r="A153" s="24"/>
+      <c r="B153" s="24"/>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D41">

</xml_diff>